<commit_message>
[ADD] Row of profile_survey in DB_tables_schema.xlsx
</commit_message>
<xml_diff>
--- a/DataFiles/DB_tables_schema (1).xlsx
+++ b/DataFiles/DB_tables_schema (1).xlsx
@@ -4,7 +4,7 @@
   <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet r:id="rId1" sheetId="1" name="profile_survey"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="367" uniqueCount="137">
   <si>
     <t>id</t>
   </si>
@@ -274,6 +274,9 @@
     <t>example</t>
   </si>
   <si>
+    <t>Is_company?</t>
+  </si>
+  <si>
     <t>Name</t>
   </si>
   <si>
@@ -287,6 +290,9 @@
   </si>
   <si>
     <t>This won't be displayed publicly, we only use this to match you with the perfect offers for you</t>
+  </si>
+  <si>
+    <t>FALSO</t>
   </si>
   <si>
     <t>Last Name</t>
@@ -393,6 +399,9 @@
   </si>
   <si>
     <t>please enter your phone number without country code</t>
+  </si>
+  <si>
+    <t>VERDADERO</t>
   </si>
   <si>
     <t>phone verification</t>
@@ -430,7 +439,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -442,6 +451,12 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -507,10 +522,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
+      <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -519,9 +534,9 @@
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
+      <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
@@ -536,7 +551,7 @@
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
@@ -552,6 +567,9 @@
       <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
   </cellXfs>
@@ -858,7 +876,7 @@
   </sheetPr>
   <dimension ref="A1:J37"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -871,7 +889,7 @@
     <col min="7" max="7" style="9" width="17.576428571428572" customWidth="1" bestFit="1"/>
     <col min="8" max="8" style="4" width="68.86214285714286" customWidth="1" bestFit="1"/>
     <col min="9" max="9" style="9" width="14.290714285714287" customWidth="1" bestFit="1"/>
-    <col min="10" max="10" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="10" max="10" style="16" width="13.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
@@ -880,11 +898,11 @@
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
-      <c r="F1" s="10"/>
+      <c r="F1" s="5"/>
       <c r="G1" s="5"/>
       <c r="H1" s="1"/>
       <c r="I1" s="5"/>
-      <c r="J1" s="1"/>
+      <c r="J1" s="10"/>
     </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
       <c r="A2" s="6" t="s">
@@ -896,11 +914,11 @@
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
-      <c r="F2" s="10"/>
+      <c r="F2" s="5"/>
       <c r="G2" s="5"/>
       <c r="H2" s="1"/>
       <c r="I2" s="5"/>
-      <c r="J2" s="1"/>
+      <c r="J2" s="10"/>
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
       <c r="A3" s="6" t="s">
@@ -912,11 +930,11 @@
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
-      <c r="F3" s="10"/>
+      <c r="F3" s="5"/>
       <c r="G3" s="5"/>
       <c r="H3" s="1"/>
       <c r="I3" s="5"/>
-      <c r="J3" s="1"/>
+      <c r="J3" s="10"/>
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
       <c r="A4" s="6" t="s">
@@ -928,11 +946,11 @@
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
-      <c r="F4" s="10"/>
+      <c r="F4" s="5"/>
       <c r="G4" s="5"/>
       <c r="H4" s="1"/>
       <c r="I4" s="5"/>
-      <c r="J4" s="1"/>
+      <c r="J4" s="10"/>
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
       <c r="A5" s="6" t="s">
@@ -950,7 +968,7 @@
       <c r="G5" s="5"/>
       <c r="H5" s="1"/>
       <c r="I5" s="5"/>
-      <c r="J5" s="1"/>
+      <c r="J5" s="10"/>
     </row>
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
       <c r="A6" s="6" t="s">
@@ -972,7 +990,7 @@
       <c r="I6" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="J6" s="1"/>
+      <c r="J6" s="10"/>
     </row>
     <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
       <c r="A7" s="6" t="s">
@@ -998,7 +1016,7 @@
         <v>81</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
       <c r="A8" s="6" t="s">
         <v>78</v>
       </c>
@@ -1032,11 +1050,11 @@
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
-      <c r="F9" s="10"/>
+      <c r="F9" s="5"/>
       <c r="G9" s="5"/>
       <c r="H9" s="1"/>
       <c r="I9" s="5"/>
-      <c r="J9" s="1"/>
+      <c r="J9" s="10"/>
     </row>
     <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
       <c r="A10" s="6" t="s">
@@ -1048,11 +1066,11 @@
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
-      <c r="F10" s="10"/>
+      <c r="F10" s="5"/>
       <c r="G10" s="5"/>
       <c r="H10" s="1"/>
       <c r="I10" s="5"/>
-      <c r="J10" s="1"/>
+      <c r="J10" s="10"/>
     </row>
     <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
       <c r="A11" s="6" t="s">
@@ -1064,11 +1082,11 @@
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
-      <c r="F11" s="10"/>
+      <c r="F11" s="5"/>
       <c r="G11" s="5"/>
       <c r="H11" s="1"/>
       <c r="I11" s="5"/>
-      <c r="J11" s="1"/>
+      <c r="J11" s="10"/>
     </row>
     <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
       <c r="A12" s="6"/>
@@ -1076,11 +1094,11 @@
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
-      <c r="F12" s="10"/>
+      <c r="F12" s="5"/>
       <c r="G12" s="5"/>
       <c r="H12" s="1"/>
       <c r="I12" s="5"/>
-      <c r="J12" s="1"/>
+      <c r="J12" s="10"/>
     </row>
     <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75">
       <c r="A13" s="6"/>
@@ -1088,23 +1106,23 @@
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
-      <c r="F13" s="10"/>
+      <c r="F13" s="5"/>
       <c r="G13" s="5"/>
       <c r="H13" s="1"/>
       <c r="I13" s="5"/>
-      <c r="J13" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75">
+      <c r="J13" s="10"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5">
       <c r="A14" s="6"/>
       <c r="B14" s="2"/>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
-      <c r="F14" s="10"/>
+      <c r="F14" s="5"/>
       <c r="G14" s="5"/>
       <c r="H14" s="1"/>
       <c r="I14" s="5"/>
-      <c r="J14" s="1"/>
+      <c r="J14" s="10"/>
     </row>
     <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18.75">
       <c r="A15" s="5"/>
@@ -1112,11 +1130,11 @@
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
-      <c r="F15" s="10"/>
+      <c r="F15" s="5"/>
       <c r="G15" s="5"/>
       <c r="H15" s="1"/>
       <c r="I15" s="5"/>
-      <c r="J15" s="1"/>
+      <c r="J15" s="10"/>
     </row>
     <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="18.75">
       <c r="A16" s="7" t="s">
@@ -1126,13 +1144,13 @@
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
-      <c r="F16" s="10"/>
+      <c r="F16" s="5"/>
       <c r="G16" s="5"/>
       <c r="H16" s="1"/>
       <c r="I16" s="5"/>
-      <c r="J16" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="18.75">
+      <c r="J16" s="10"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="19.5">
       <c r="A17" s="6" t="s">
         <v>2</v>
       </c>
@@ -1160,23 +1178,25 @@
       <c r="I17" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="J17" s="1"/>
+      <c r="J17" s="10" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="18.75">
       <c r="A18" s="11">
         <v>1</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="F18" s="7" t="s">
         <v>34</v>
@@ -1185,28 +1205,30 @@
         <v>1</v>
       </c>
       <c r="H18" s="3" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="I18" s="11">
         <v>1</v>
       </c>
-      <c r="J18" s="1"/>
+      <c r="J18" s="10" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="18.75">
       <c r="A19" s="11">
         <v>2</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="F19" s="7" t="s">
         <v>34</v>
@@ -1215,56 +1237,60 @@
         <v>1</v>
       </c>
       <c r="H19" s="3" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="I19" s="11">
         <v>1</v>
       </c>
-      <c r="J19" s="1"/>
+      <c r="J19" s="10" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="18.75">
       <c r="A20" s="7"/>
       <c r="B20" s="3" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="F20" s="7" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="G20" s="11">
         <v>4</v>
       </c>
       <c r="H20" s="3" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="I20" s="11">
         <v>1</v>
       </c>
-      <c r="J20" s="1"/>
+      <c r="J20" s="10" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="18.75">
       <c r="A21" s="11">
         <v>3</v>
       </c>
       <c r="B21" s="12" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="C21" s="12" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="D21" s="12" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="E21" s="12" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="F21" s="13" t="s">
         <v>34</v>
@@ -1273,28 +1299,30 @@
         <v>3</v>
       </c>
       <c r="H21" s="12" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="I21" s="14">
         <v>1</v>
       </c>
-      <c r="J21" s="1"/>
+      <c r="J21" s="10" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="18.75">
       <c r="A22" s="11">
         <v>4</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="F22" s="7" t="s">
         <v>34</v>
@@ -1303,28 +1331,30 @@
         <v>2</v>
       </c>
       <c r="H22" s="3" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="I22" s="11">
         <v>1</v>
       </c>
-      <c r="J22" s="1"/>
+      <c r="J22" s="10" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="18.75">
       <c r="A23" s="11">
         <v>5</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="F23" s="7" t="s">
         <v>34</v>
@@ -1333,28 +1363,30 @@
         <v>2</v>
       </c>
       <c r="H23" s="3" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="I23" s="11">
         <v>1</v>
       </c>
-      <c r="J23" s="1"/>
+      <c r="J23" s="10" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="18.75">
       <c r="A24" s="11">
         <v>6</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="F24" s="7" t="s">
         <v>34</v>
@@ -1363,28 +1395,30 @@
         <v>2</v>
       </c>
       <c r="H24" s="3" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="I24" s="11">
         <v>1</v>
       </c>
-      <c r="J24" s="1"/>
+      <c r="J24" s="10" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="18.75">
       <c r="A25" s="11">
         <v>7</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="F25" s="7" t="s">
         <v>34</v>
@@ -1393,28 +1427,30 @@
         <v>1</v>
       </c>
       <c r="H25" s="3" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="I25" s="11">
         <v>1</v>
       </c>
-      <c r="J25" s="1"/>
+      <c r="J25" s="10" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="18.75">
       <c r="A26" s="11">
         <v>8</v>
       </c>
       <c r="B26" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="D26" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="C26" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="D26" s="3" t="s">
-        <v>102</v>
-      </c>
       <c r="E26" s="3" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="F26" s="7" t="s">
         <v>34</v>
@@ -1423,28 +1459,30 @@
         <v>1</v>
       </c>
       <c r="H26" s="3" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="I26" s="11">
         <v>1</v>
       </c>
-      <c r="J26" s="1"/>
+      <c r="J26" s="10" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="18.75">
       <c r="A27" s="11">
         <v>9</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="F27" s="7" t="s">
         <v>34</v>
@@ -1453,28 +1491,30 @@
         <v>1</v>
       </c>
       <c r="H27" s="3" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="I27" s="11">
         <v>1</v>
       </c>
-      <c r="J27" s="1"/>
+      <c r="J27" s="10" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="18.75">
       <c r="A28" s="11">
         <v>10</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="F28" s="7" t="s">
         <v>34</v>
@@ -1483,28 +1523,30 @@
         <v>1</v>
       </c>
       <c r="H28" s="3" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="I28" s="11">
         <v>1</v>
       </c>
-      <c r="J28" s="1"/>
+      <c r="J28" s="10" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="18.75">
       <c r="A29" s="11">
         <v>11</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="F29" s="7" t="s">
         <v>34</v>
@@ -1513,28 +1555,30 @@
         <v>2</v>
       </c>
       <c r="H29" s="3" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="I29" s="11">
         <v>1</v>
       </c>
-      <c r="J29" s="1"/>
+      <c r="J29" s="10" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="18.75">
       <c r="A30" s="11">
         <v>12</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="F30" s="7" t="s">
         <v>34</v>
@@ -1543,28 +1587,30 @@
         <v>1</v>
       </c>
       <c r="H30" s="3" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="I30" s="11">
         <v>1</v>
       </c>
-      <c r="J30" s="1"/>
+      <c r="J30" s="10" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="18.75">
       <c r="A31" s="11">
         <v>13</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="F31" s="7" t="s">
         <v>34</v>
@@ -1573,58 +1619,62 @@
         <v>1</v>
       </c>
       <c r="H31" s="3" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="I31" s="11">
         <v>1</v>
       </c>
-      <c r="J31" s="1"/>
+      <c r="J31" s="10" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="18.75">
       <c r="A32" s="11">
         <v>14</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="F32" s="7" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="G32" s="11">
         <v>6</v>
       </c>
       <c r="H32" s="3" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="I32" s="11">
         <v>1</v>
       </c>
-      <c r="J32" s="1"/>
+      <c r="J32" s="10" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="18.75">
       <c r="A33" s="11">
         <v>15</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="F33" s="7" t="s">
         <v>34</v>
@@ -1633,28 +1683,30 @@
         <v>1</v>
       </c>
       <c r="H33" s="3" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="I33" s="11">
         <v>1</v>
       </c>
-      <c r="J33" s="1"/>
+      <c r="J33" s="10" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="18.75">
       <c r="A34" s="11">
         <v>17</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="F34" s="7" t="s">
         <v>34</v>
@@ -1663,28 +1715,30 @@
         <v>2</v>
       </c>
       <c r="H34" s="3" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="I34" s="11">
         <v>1</v>
       </c>
-      <c r="J34" s="1"/>
+      <c r="J34" s="10" t="s">
+        <v>126</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="18.75">
       <c r="A35" s="11">
         <v>18</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="F35" s="7" t="s">
         <v>34</v>
@@ -1693,66 +1747,72 @@
         <v>2</v>
       </c>
       <c r="H35" s="3" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="I35" s="11">
         <v>1</v>
       </c>
-      <c r="J35" s="1"/>
+      <c r="J35" s="10" t="s">
+        <v>126</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="18.75">
       <c r="A36" s="11">
         <v>19</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="F36" s="7" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="G36" s="7"/>
       <c r="H36" s="3"/>
       <c r="I36" s="7"/>
-      <c r="J36" s="1"/>
+      <c r="J36" s="10" t="s">
+        <v>126</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="18.75">
       <c r="A37" s="11">
         <v>20</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="F37" s="7" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="G37" s="11">
         <v>4</v>
       </c>
       <c r="H37" s="3" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="I37" s="11">
         <v>1</v>
       </c>
-      <c r="J37" s="1"/>
+      <c r="J37" s="10" t="s">
+        <v>126</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1766,7 +1826,7 @@
   </sheetPr>
   <dimension ref="A1:I37"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>